<commit_message>
lots of work on landings data
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CE85DC-9CA8-FD4C-92BF-96F178623070}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806ECBB3-5825-254C-8EB0-C6C6BC84B990}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22020" yWindow="460" windowWidth="22380" windowHeight="22060" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
+    <workbookView xWindow="3220" yWindow="460" windowWidth="22380" windowHeight="15540" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
lots of work on port-level landings
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0064AEB-6DEF-7143-81DC-1F2690DF64AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D63FA6-CF4F-7A4C-9A89-1CFB03FC7E37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="720" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
+    <workbookView xWindow="22860" yWindow="2360" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
   <dimension ref="A2:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="C20" sqref="B20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
a few edits to port-level data
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D63FA6-CF4F-7A4C-9A89-1CFB03FC7E37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C1D746-A8D6-7243-8BFB-D239FDB78906}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22860" yWindow="2360" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
+    <workbookView xWindow="17760" yWindow="4640" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
   <dimension ref="A2:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="B20:C20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
worked on PACFIN data
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C1D746-A8D6-7243-8BFB-D239FDB78906}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCD8716-A52C-4840-82F2-E575E55DB7BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17760" yWindow="4640" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
+    <workbookView xWindow="23040" yWindow="4320" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
   <dimension ref="A2:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
by waters data and more
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCD8716-A52C-4840-82F2-E575E55DB7BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D7513C-0BF5-7B45-AFEF-3D2620A9B570}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23040" yWindow="4320" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
+    <workbookView xWindow="14820" yWindow="2180" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
   <dimension ref="A2:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
lots of misc work
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D7513C-0BF5-7B45-AFEF-3D2620A9B570}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C237F794-F342-8246-A7AB-33242098863E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14820" yWindow="2180" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="A2:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
a ridiculous amount of work
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/fish_bulletin_landings_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C237F794-F342-8246-A7AB-33242098863E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5460172-B141-9A43-A5AF-74CEE0F16CE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14820" yWindow="2180" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
+    <workbookView xWindow="24520" yWindow="2100" windowWidth="24800" windowHeight="22640" xr2:uid="{A8352594-68AE-3D4A-A616-D815EB4A4B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
   <dimension ref="A2:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>